<commit_message>
Added plotting functions to michigan sensitivity
</commit_message>
<xml_diff>
--- a/results/Michigan_Scenario0.xlsx
+++ b/results/Michigan_Scenario0.xlsx
@@ -487,7 +487,7 @@
         <v>157201637.8935993</v>
       </c>
       <c r="O2">
-        <v>997231391.23026</v>
+        <v>997231391.2302537</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -581,7 +581,7 @@
         <v>112283218.2154742</v>
       </c>
       <c r="O4">
-        <v>884835983.9680685</v>
+        <v>884835983.953926</v>
       </c>
     </row>
   </sheetData>

</xml_diff>